<commit_message>
Simplificando a coleta de dados e removendo comentários
</commit_message>
<xml_diff>
--- a/planilha.xlsx
+++ b/planilha.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">6° Termo</t>
   </si>
   <si>
-    <t xml:space="preserve">Tamanho população: 10</t>
+    <t xml:space="preserve">Tamanho população: 100</t>
   </si>
   <si>
     <t xml:space="preserve">Logica de programação / Hilário / 4</t>
@@ -295,10 +295,10 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.11"/>

</xml_diff>

<commit_message>
Adicionando coleta do número de professores
</commit_message>
<xml_diff>
--- a/planilha.xlsx
+++ b/planilha.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t xml:space="preserve">Configurações</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">6° Termo</t>
   </si>
   <si>
-    <t xml:space="preserve">Tamanho população: 100</t>
+    <t xml:space="preserve">Tamanho população: 10000</t>
   </si>
   <si>
     <t xml:space="preserve">Logica de programação / Hilário / 4</t>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t xml:space="preserve">Inteligência artificial / Favan / 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Número de professores: 18</t>
   </si>
   <si>
     <t xml:space="preserve">Produção vegetal de culturas anuais / Élvio / 2</t>
@@ -294,11 +297,11 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.11"/>
@@ -306,6 +309,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="49.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="56.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="46.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="43.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -424,59 +428,62 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>35</v>
+      </c>
       <c r="B6" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C9" s="4"/>
     </row>

</xml_diff>

<commit_message>
Adicionando coleta de dados: disponibilidade dos professores no json e número de professores no excel
</commit_message>
<xml_diff>
--- a/planilha.xlsx
+++ b/planilha.xlsx
@@ -127,7 +127,7 @@
     <t xml:space="preserve">Inteligência artificial / Favan / 4</t>
   </si>
   <si>
-    <t xml:space="preserve">Número de professores: 18</t>
+    <t xml:space="preserve">Número de professores: 5</t>
   </si>
   <si>
     <t xml:space="preserve">Produção vegetal de culturas anuais / Élvio / 2</t>
@@ -309,7 +309,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="49.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="56.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="46.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="43.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="43.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Corrigindo professores json e adicionando verificação de professores
</commit_message>
<xml_diff>
--- a/planilha.xlsx
+++ b/planilha.xlsx
@@ -118,7 +118,7 @@
     <t xml:space="preserve">Estatística / Deise / 4</t>
   </si>
   <si>
-    <t xml:space="preserve">Algoritmos Avançados / Adriano Nakamura / 6</t>
+    <t xml:space="preserve">Algoritmos Avançados / Adriano / 6</t>
   </si>
   <si>
     <t xml:space="preserve">Banco de dados No-SQL / Querino / 4</t>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">Inteligência artificial / Favan / 4</t>
   </si>
   <si>
-    <t xml:space="preserve">Número de professores: 5</t>
+    <t xml:space="preserve">Número de professores: 16</t>
   </si>
   <si>
     <t xml:space="preserve">Produção vegetal de culturas anuais / Élvio / 2</t>
@@ -157,7 +157,7 @@
     <t xml:space="preserve">Geometria analítica / Marçal / 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Redes de computadores / Adriano Nakamura / 4</t>
+    <t xml:space="preserve">Redes de computadores / Adriano / 4</t>
   </si>
   <si>
     <t xml:space="preserve">Inglês V / Eloiza / 2</t>
@@ -297,11 +297,11 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.11"/>
@@ -309,7 +309,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="49.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="56.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="46.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="43.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="43.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.53"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Adicionando fitness de disponibilidade de professores e alterando o json
</commit_message>
<xml_diff>
--- a/planilha.xlsx
+++ b/planilha.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">6° Termo</t>
   </si>
   <si>
-    <t xml:space="preserve">Tamanho população: 10000</t>
+    <t xml:space="preserve">Tamanho população: 100</t>
   </si>
   <si>
     <t xml:space="preserve">Logica de programação / Hilário / 4</t>
@@ -298,10 +298,10 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.11"/>

</xml_diff>

<commit_message>
Adicionando geração da população inicial sem conflito
</commit_message>
<xml_diff>
--- a/planilha.xlsx
+++ b/planilha.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">6° Termo</t>
   </si>
   <si>
-    <t xml:space="preserve">Tamanho população: 1000</t>
+    <t xml:space="preserve">Tamanho população: 100</t>
   </si>
   <si>
     <t xml:space="preserve">Logica de programação / Hilário / 4</t>
@@ -301,7 +301,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.11"/>

</xml_diff>

<commit_message>
Subindo fitness function corrigida
</commit_message>
<xml_diff>
--- a/planilha.xlsx
+++ b/planilha.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">6° Termo</t>
   </si>
   <si>
-    <t xml:space="preserve">Tamanho população: 100</t>
+    <t xml:space="preserve">Tamanho população: 1000</t>
   </si>
   <si>
     <t xml:space="preserve">Logica de programação / Hilário / 4</t>
@@ -301,7 +301,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.11"/>

</xml_diff>

<commit_message>
Adicionando função de geração da roleta
</commit_message>
<xml_diff>
--- a/planilha.xlsx
+++ b/planilha.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">6° Termo</t>
   </si>
   <si>
-    <t xml:space="preserve">Tamanho população: 1000</t>
+    <t xml:space="preserve">Tamanho população: 10</t>
   </si>
   <si>
     <t xml:space="preserve">Logica de programação / Hilário / 4</t>
@@ -301,7 +301,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.11"/>

</xml_diff>

<commit_message>
Subindo algoritmo com reprodução
</commit_message>
<xml_diff>
--- a/planilha.xlsx
+++ b/planilha.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t xml:space="preserve">Configurações</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">6° Termo</t>
   </si>
   <si>
-    <t xml:space="preserve">Tamanho população: 10</t>
+    <t xml:space="preserve">Tamanho população: 100</t>
   </si>
   <si>
     <t xml:space="preserve">Logica de programação / Hilário / 4</t>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t xml:space="preserve">Aprendizado de máquina / Favan / 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Número de gerações: 10000</t>
   </si>
   <si>
     <t xml:space="preserve">Inglês I / Eloiza / 2</t>
@@ -298,10 +301,10 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.11"/>
@@ -452,46 +455,49 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>42</v>
+      </c>
       <c r="B7" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C9" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>

</xml_diff>

<commit_message>
Corrigindo erro de encoding windows
</commit_message>
<xml_diff>
--- a/planilha.xlsx
+++ b/planilha.xlsx
@@ -148,7 +148,7 @@
     <t xml:space="preserve">Aprendizado de máquina / Favan / 4</t>
   </si>
   <si>
-    <t xml:space="preserve">Número de gerações: 5000</t>
+    <t xml:space="preserve">Número de gerações: 50000</t>
   </si>
   <si>
     <t xml:space="preserve">Inglês I / Eloiza / 2</t>
@@ -304,7 +304,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="47.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.11"/>

</xml_diff>